<commit_message>
fix style cells from .xlsx Patterns
</commit_message>
<xml_diff>
--- a/PatternFinalReport.xlsx
+++ b/PatternFinalReport.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stepankonasenko/Documents/javaWork/практика-обучение/SpringTestReportsBot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{747A3816-98E1-6C4B-ACD0-9C9E612CDA52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A56784A7-DFD4-2245-8168-905ADC780CB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28420" windowHeight="15980" xr2:uid="{082E3804-15BA-084E-9FB2-E5566443FF13}"/>
   </bookViews>
@@ -435,7 +435,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -449,9 +449,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -472,16 +469,10 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -490,22 +481,10 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -523,16 +502,10 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
@@ -557,6 +530,39 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -6629,8 +6635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAEA3E71-2659-D644-9294-867F3A6297D1}">
   <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="61" zoomScaleNormal="43" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="44" zoomScaleNormal="43" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6639,204 +6645,204 @@
     <col min="2" max="10" width="40.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="10" customFormat="1" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+    <row r="1" spans="1:10" s="9" customFormat="1" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="39"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="30"/>
     </row>
     <row r="2" spans="1:10" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="14">
-        <v>0</v>
-      </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="16"/>
+      <c r="A2" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="34">
+        <v>0</v>
+      </c>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="14"/>
     </row>
     <row r="3" spans="1:10" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="17">
-        <v>0</v>
-      </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="19"/>
+      <c r="B3" s="35">
+        <v>0</v>
+      </c>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="16"/>
     </row>
     <row r="4" spans="1:10" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="20">
-        <v>0</v>
-      </c>
-      <c r="C4" s="29" t="s">
+      <c r="B4" s="36">
+        <v>0</v>
+      </c>
+      <c r="C4" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="31">
-        <v>0</v>
-      </c>
-      <c r="E4" s="30" t="s">
+      <c r="D4" s="37">
+        <v>0</v>
+      </c>
+      <c r="E4" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="F4" s="31">
-        <v>0</v>
-      </c>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="21"/>
-      <c r="J4" s="22"/>
+      <c r="F4" s="37">
+        <v>0</v>
+      </c>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="18"/>
     </row>
     <row r="5" spans="1:10" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="37" t="s">
+      <c r="A5" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="38"/>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="38"/>
-      <c r="I5" s="38"/>
-      <c r="J5" s="39"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="29"/>
+      <c r="J5" s="30"/>
     </row>
     <row r="6" spans="1:10" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="14">
-        <v>0</v>
-      </c>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="16"/>
+      <c r="B6" s="34">
+        <v>0</v>
+      </c>
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="38"/>
+      <c r="H6" s="38"/>
+      <c r="I6" s="38"/>
+      <c r="J6" s="39"/>
     </row>
     <row r="7" spans="1:10" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="23">
-        <v>0</v>
-      </c>
-      <c r="C7" s="24">
-        <v>0</v>
-      </c>
-      <c r="D7" s="24">
-        <v>0</v>
-      </c>
-      <c r="E7" s="24">
-        <v>0</v>
-      </c>
-      <c r="F7" s="24">
-        <v>0</v>
-      </c>
-      <c r="G7" s="24">
-        <v>0</v>
-      </c>
-      <c r="H7" s="24">
-        <v>0</v>
-      </c>
-      <c r="I7" s="24">
-        <v>0</v>
-      </c>
-      <c r="J7" s="25">
+      <c r="B7" s="40">
+        <v>0</v>
+      </c>
+      <c r="C7" s="41">
+        <v>0</v>
+      </c>
+      <c r="D7" s="41">
+        <v>0</v>
+      </c>
+      <c r="E7" s="41">
+        <v>0</v>
+      </c>
+      <c r="F7" s="41">
+        <v>0</v>
+      </c>
+      <c r="G7" s="41">
+        <v>0</v>
+      </c>
+      <c r="H7" s="41">
+        <v>0</v>
+      </c>
+      <c r="I7" s="41">
+        <v>0</v>
+      </c>
+      <c r="J7" s="42">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="37" t="s">
+      <c r="A8" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="38"/>
-      <c r="C8" s="38"/>
-      <c r="D8" s="38"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="38"/>
-      <c r="G8" s="38"/>
-      <c r="H8" s="38"/>
-      <c r="I8" s="38"/>
-      <c r="J8" s="39"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="29"/>
+      <c r="I8" s="29"/>
+      <c r="J8" s="30"/>
     </row>
     <row r="9" spans="1:10" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="27" t="s">
+      <c r="A9" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="34">
+      <c r="B9" s="43">
         <f>A30</f>
         <v>0</v>
       </c>
-      <c r="C9" s="34">
+      <c r="C9" s="43">
         <f>A31</f>
         <v>0</v>
       </c>
-      <c r="D9" s="34">
+      <c r="D9" s="43">
         <f>A32</f>
         <v>0</v>
       </c>
-      <c r="E9" s="34">
+      <c r="E9" s="43">
         <f>A33</f>
         <v>0</v>
       </c>
-      <c r="F9" s="34">
+      <c r="F9" s="43">
         <f>A34</f>
         <v>0</v>
       </c>
-      <c r="G9" s="34">
+      <c r="G9" s="43">
         <f>A35</f>
         <v>0</v>
       </c>
-      <c r="H9" s="28"/>
-      <c r="I9" s="28"/>
-      <c r="J9" s="28"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="21"/>
     </row>
     <row r="10" spans="1:10" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="6">
-        <v>0</v>
-      </c>
-      <c r="C10" s="6">
-        <v>0</v>
-      </c>
-      <c r="D10" s="6">
-        <v>0</v>
-      </c>
-      <c r="E10" s="6">
-        <v>0</v>
-      </c>
-      <c r="F10" s="6">
-        <v>0</v>
-      </c>
-      <c r="G10" s="6">
+      <c r="B10" s="24">
+        <v>0</v>
+      </c>
+      <c r="C10" s="24">
+        <v>0</v>
+      </c>
+      <c r="D10" s="24">
+        <v>0</v>
+      </c>
+      <c r="E10" s="24">
+        <v>0</v>
+      </c>
+      <c r="F10" s="24">
+        <v>0</v>
+      </c>
+      <c r="G10" s="24">
         <v>0</v>
       </c>
       <c r="H10" s="6"/>
@@ -6844,25 +6850,25 @@
       <c r="J10" s="6"/>
     </row>
     <row r="11" spans="1:10" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="7">
-        <v>0</v>
-      </c>
-      <c r="C11" s="7">
-        <v>0</v>
-      </c>
-      <c r="D11" s="6">
-        <v>0</v>
-      </c>
-      <c r="E11" s="6">
-        <v>0</v>
-      </c>
-      <c r="F11" s="6">
-        <v>0</v>
-      </c>
-      <c r="G11" s="6">
+      <c r="B11" s="44">
+        <v>0</v>
+      </c>
+      <c r="C11" s="44">
+        <v>0</v>
+      </c>
+      <c r="D11" s="24">
+        <v>0</v>
+      </c>
+      <c r="E11" s="24">
+        <v>0</v>
+      </c>
+      <c r="F11" s="24">
+        <v>0</v>
+      </c>
+      <c r="G11" s="24">
         <v>0</v>
       </c>
       <c r="H11" s="6"/>
@@ -6870,14 +6876,14 @@
       <c r="J11" s="6"/>
     </row>
     <row r="12" spans="1:10" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="37" t="s">
+      <c r="A12" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="38"/>
-      <c r="C12" s="39"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="30"/>
     </row>
     <row r="13" spans="1:10" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="26"/>
+      <c r="A13" s="19"/>
       <c r="B13" s="5" t="s">
         <v>15</v>
       </c>
@@ -6889,13 +6895,13 @@
       </c>
     </row>
     <row r="14" spans="1:10" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="27" t="s">
+      <c r="A14" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="6">
-        <v>0</v>
-      </c>
-      <c r="C14" s="6">
+      <c r="B14" s="24">
+        <v>0</v>
+      </c>
+      <c r="C14" s="24">
         <v>0</v>
       </c>
       <c r="D14">
@@ -6904,13 +6910,13 @@
       </c>
     </row>
     <row r="15" spans="1:10" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="6">
-        <v>0</v>
-      </c>
-      <c r="C15" s="6">
+      <c r="B15" s="24">
+        <v>0</v>
+      </c>
+      <c r="C15" s="24">
         <v>0</v>
       </c>
       <c r="D15">
@@ -6919,11 +6925,11 @@
       </c>
     </row>
     <row r="16" spans="1:10" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="40" t="s">
+      <c r="A16" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="41"/>
-      <c r="C16" s="42"/>
+      <c r="B16" s="32"/>
+      <c r="C16" s="33"/>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="1:4" ht="28" customHeight="1" x14ac:dyDescent="0.2">
@@ -6942,10 +6948,10 @@
       <c r="A18" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="6">
-        <v>0</v>
-      </c>
-      <c r="C18" s="6">
+      <c r="B18" s="24">
+        <v>0</v>
+      </c>
+      <c r="C18" s="24">
         <v>0</v>
       </c>
       <c r="D18">
@@ -6957,10 +6963,10 @@
       <c r="A19" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="6">
-        <v>0</v>
-      </c>
-      <c r="C19" s="6">
+      <c r="B19" s="24">
+        <v>0</v>
+      </c>
+      <c r="C19" s="24">
         <v>0</v>
       </c>
       <c r="D19">
@@ -6972,10 +6978,10 @@
       <c r="A20" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="7">
-        <v>0</v>
-      </c>
-      <c r="C20" s="7">
+      <c r="B20" s="44">
+        <v>0</v>
+      </c>
+      <c r="C20" s="44">
         <v>0</v>
       </c>
       <c r="D20">
@@ -6984,15 +6990,15 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="40" t="s">
+      <c r="A21" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="41"/>
-      <c r="C21" s="42"/>
+      <c r="B21" s="32"/>
+      <c r="C21" s="33"/>
       <c r="D21" s="1"/>
     </row>
     <row r="22" spans="1:4" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="8"/>
+      <c r="A22" s="7"/>
       <c r="B22" s="5" t="s">
         <v>15</v>
       </c>
@@ -7004,13 +7010,13 @@
       </c>
     </row>
     <row r="23" spans="1:4" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="9" t="s">
+      <c r="A23" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B23" s="6">
-        <v>0</v>
-      </c>
-      <c r="C23" s="6">
+      <c r="B23" s="24">
+        <v>0</v>
+      </c>
+      <c r="C23" s="24">
         <v>0</v>
       </c>
       <c r="D23">
@@ -7019,13 +7025,13 @@
       </c>
     </row>
     <row r="24" spans="1:4" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="9" t="s">
+      <c r="A24" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B24" s="6">
-        <v>0</v>
-      </c>
-      <c r="C24" s="6">
+      <c r="B24" s="24">
+        <v>0</v>
+      </c>
+      <c r="C24" s="24">
         <v>0</v>
       </c>
       <c r="D24">
@@ -7034,13 +7040,13 @@
       </c>
     </row>
     <row r="25" spans="1:4" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="9" t="s">
+      <c r="A25" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B25" s="6">
-        <v>0</v>
-      </c>
-      <c r="C25" s="6">
+      <c r="B25" s="24">
+        <v>0</v>
+      </c>
+      <c r="C25" s="24">
         <v>0</v>
       </c>
       <c r="D25">
@@ -7049,13 +7055,13 @@
       </c>
     </row>
     <row r="26" spans="1:4" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="9" t="s">
+      <c r="A26" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B26" s="6">
-        <v>0</v>
-      </c>
-      <c r="C26" s="6">
+      <c r="B26" s="24">
+        <v>0</v>
+      </c>
+      <c r="C26" s="24">
         <v>0</v>
       </c>
       <c r="D26">
@@ -7064,13 +7070,13 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="9" t="s">
+      <c r="A27" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B27" s="6">
-        <v>0</v>
-      </c>
-      <c r="C27" s="6">
+      <c r="B27" s="24">
+        <v>0</v>
+      </c>
+      <c r="C27" s="24">
         <v>0</v>
       </c>
       <c r="D27">
@@ -7079,11 +7085,11 @@
       </c>
     </row>
     <row r="28" spans="1:4" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="37" t="s">
+      <c r="A28" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="38"/>
-      <c r="C28" s="39"/>
+      <c r="B28" s="29"/>
+      <c r="C28" s="30"/>
     </row>
     <row r="29" spans="1:4" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
@@ -7095,18 +7101,18 @@
       <c r="C29" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D29" s="33" t="s">
+      <c r="D29" s="25" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="6">
-        <v>0</v>
-      </c>
-      <c r="B30" s="6">
-        <v>0</v>
-      </c>
-      <c r="C30" s="6">
+      <c r="A30" s="24">
+        <v>0</v>
+      </c>
+      <c r="B30" s="24">
+        <v>0</v>
+      </c>
+      <c r="C30" s="24">
         <v>0</v>
       </c>
       <c r="D30">
@@ -7115,13 +7121,13 @@
       </c>
     </row>
     <row r="31" spans="1:4" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="34">
-        <v>0</v>
-      </c>
-      <c r="B31" s="6">
-        <v>0</v>
-      </c>
-      <c r="C31" s="6">
+      <c r="A31" s="43">
+        <v>0</v>
+      </c>
+      <c r="B31" s="24">
+        <v>0</v>
+      </c>
+      <c r="C31" s="24">
         <v>0</v>
       </c>
       <c r="D31">
@@ -7130,13 +7136,13 @@
       </c>
     </row>
     <row r="32" spans="1:4" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="34">
-        <v>0</v>
-      </c>
-      <c r="B32" s="6">
-        <v>0</v>
-      </c>
-      <c r="C32" s="6">
+      <c r="A32" s="43">
+        <v>0</v>
+      </c>
+      <c r="B32" s="24">
+        <v>0</v>
+      </c>
+      <c r="C32" s="24">
         <v>0</v>
       </c>
       <c r="D32">
@@ -7145,13 +7151,13 @@
       </c>
     </row>
     <row r="33" spans="1:4" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="6">
-        <v>0</v>
-      </c>
-      <c r="B33" s="6">
-        <v>0</v>
-      </c>
-      <c r="C33" s="6">
+      <c r="A33" s="24">
+        <v>0</v>
+      </c>
+      <c r="B33" s="24">
+        <v>0</v>
+      </c>
+      <c r="C33" s="24">
         <v>0</v>
       </c>
       <c r="D33">
@@ -7160,13 +7166,13 @@
       </c>
     </row>
     <row r="34" spans="1:4" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="6">
-        <v>0</v>
-      </c>
-      <c r="B34" s="6">
-        <v>0</v>
-      </c>
-      <c r="C34" s="6">
+      <c r="A34" s="24">
+        <v>0</v>
+      </c>
+      <c r="B34" s="24">
+        <v>0</v>
+      </c>
+      <c r="C34" s="24">
         <v>0</v>
       </c>
       <c r="D34">
@@ -7175,13 +7181,13 @@
       </c>
     </row>
     <row r="35" spans="1:4" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="6">
-        <v>0</v>
-      </c>
-      <c r="B35" s="6">
-        <v>0</v>
-      </c>
-      <c r="C35" s="6">
+      <c r="A35" s="24">
+        <v>0</v>
+      </c>
+      <c r="B35" s="24">
+        <v>0</v>
+      </c>
+      <c r="C35" s="24">
         <v>0</v>
       </c>
       <c r="D35">
@@ -7190,14 +7196,14 @@
       </c>
     </row>
     <row r="36" spans="1:4" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="32" t="s">
+      <c r="A36" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="B36" s="6">
+      <c r="B36" s="24">
         <f>SUM(B30:B35)</f>
         <v>0</v>
       </c>
-      <c r="C36" s="6">
+      <c r="C36" s="24">
         <f>SUM(C30:C35)</f>
         <v>0</v>
       </c>
@@ -7207,73 +7213,73 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="37" t="s">
+      <c r="A37" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="B37" s="38"/>
-      <c r="C37" s="39"/>
+      <c r="B37" s="29"/>
+      <c r="C37" s="30"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="35">
-        <v>0</v>
-      </c>
-      <c r="B38" s="35"/>
-      <c r="C38" s="35"/>
+      <c r="A38" s="26">
+        <v>0</v>
+      </c>
+      <c r="B38" s="26"/>
+      <c r="C38" s="26"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" s="36"/>
-      <c r="B39" s="36"/>
-      <c r="C39" s="36"/>
+      <c r="A39" s="27"/>
+      <c r="B39" s="27"/>
+      <c r="C39" s="27"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" s="36"/>
-      <c r="B40" s="36"/>
-      <c r="C40" s="36"/>
+      <c r="A40" s="27"/>
+      <c r="B40" s="27"/>
+      <c r="C40" s="27"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" s="36"/>
-      <c r="B41" s="36"/>
-      <c r="C41" s="36"/>
+      <c r="A41" s="27"/>
+      <c r="B41" s="27"/>
+      <c r="C41" s="27"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="36"/>
-      <c r="B42" s="36"/>
-      <c r="C42" s="36"/>
+      <c r="A42" s="27"/>
+      <c r="B42" s="27"/>
+      <c r="C42" s="27"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="36"/>
-      <c r="B43" s="36"/>
-      <c r="C43" s="36"/>
+      <c r="A43" s="27"/>
+      <c r="B43" s="27"/>
+      <c r="C43" s="27"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="36"/>
-      <c r="B44" s="36"/>
-      <c r="C44" s="36"/>
+      <c r="A44" s="27"/>
+      <c r="B44" s="27"/>
+      <c r="C44" s="27"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="36"/>
-      <c r="B45" s="36"/>
-      <c r="C45" s="36"/>
+      <c r="A45" s="27"/>
+      <c r="B45" s="27"/>
+      <c r="C45" s="27"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" s="36"/>
-      <c r="B46" s="36"/>
-      <c r="C46" s="36"/>
+      <c r="A46" s="27"/>
+      <c r="B46" s="27"/>
+      <c r="C46" s="27"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" s="36"/>
-      <c r="B47" s="36"/>
-      <c r="C47" s="36"/>
+      <c r="A47" s="27"/>
+      <c r="B47" s="27"/>
+      <c r="C47" s="27"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" s="36"/>
-      <c r="B48" s="36"/>
-      <c r="C48" s="36"/>
+      <c r="A48" s="27"/>
+      <c r="B48" s="27"/>
+      <c r="C48" s="27"/>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A49" s="36"/>
-      <c r="B49" s="36"/>
-      <c r="C49" s="36"/>
+      <c r="A49" s="27"/>
+      <c r="B49" s="27"/>
+      <c r="C49" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>